<commit_message>
Refactored create_daily_case lists to query_daily_case_list_data.
</commit_message>
<xml_diff>
--- a/tests/db/Final_Pretrials.xlsx
+++ b/tests/db/Final_Pretrials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justi\AppData\Local\Programs\Python\Python310\MuniEntry\tests\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08364A0F-4BE2-49FF-B71D-56A340F54C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E746EAB-BE5C-4F3B-BF69-D781FD86E29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45972" yWindow="6996" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9015" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MuniEntryPleas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="116">
   <si>
     <t>Case</t>
   </si>
@@ -161,39 +161,6 @@
   </si>
   <si>
     <t>4513.263B1</t>
-  </si>
-  <si>
-    <t>21CRB00615</t>
-  </si>
-  <si>
-    <t>21CRB00615-A</t>
-  </si>
-  <si>
-    <t>OBSTRUCT OFFICIAL BUSINESS</t>
-  </si>
-  <si>
-    <t>2921.31</t>
-  </si>
-  <si>
-    <t>M2</t>
-  </si>
-  <si>
-    <t>21CRB01597</t>
-  </si>
-  <si>
-    <t>21CRB01597-A</t>
-  </si>
-  <si>
-    <t>ANSLEY</t>
-  </si>
-  <si>
-    <t>JACOB</t>
-  </si>
-  <si>
-    <t>POSSESSION OF MARIHUANA</t>
-  </si>
-  <si>
-    <t>2925.11C3</t>
   </si>
   <si>
     <t>MALLORY</t>
@@ -874,9 +841,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A10" activeCellId="1" sqref="A9:XFD9 A10:XFD10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
@@ -1187,97 +1156,99 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="38.25">
+    <row r="9" spans="1:12" ht="25.5">
       <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="2" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="K9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" ht="38.25">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" s="1"/>
+        <v>36</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="I10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>26</v>
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="25.5">
+    <row r="11" spans="1:12" ht="38.25">
       <c r="A11" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>63</v>
+        <v>38</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>64</v>
+        <v>39</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>19</v>
@@ -1286,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>26</v>
@@ -1295,22 +1266,22 @@
     </row>
     <row r="12" spans="1:12" ht="38.25">
       <c r="A12" s="1" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>36</v>
@@ -1319,22 +1290,22 @@
         <v>19</v>
       </c>
       <c r="I12" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>26</v>
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="38.25">
+    <row r="13" spans="1:12" ht="25.5">
       <c r="A13" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>61</v>
@@ -1343,25 +1314,25 @@
         <v>62</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I13" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="L13" s="1"/>
     </row>
@@ -1370,7 +1341,7 @@
         <v>59</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>61</v>
@@ -1379,555 +1350,483 @@
         <v>62</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="I14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="25.5">
+    <row r="15" spans="1:12" ht="38.25">
       <c r="A15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="I15" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" ht="38.25">
       <c r="A16" s="1" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" ht="25.5">
+      <c r="A17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I17" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="1" t="s">
+      <c r="K17" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" ht="51">
+      <c r="A18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I18" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I16" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="1:12" ht="38.25">
-      <c r="A17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I17" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="L17" s="1"/>
-    </row>
-    <row r="18" spans="1:12" ht="38.25">
-      <c r="A18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I18" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="L18" s="1"/>
     </row>
     <row r="19" spans="1:12" ht="25.5">
       <c r="A19" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="G19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I19" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12" ht="25.5">
+      <c r="A20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="D20" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I19" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L19" s="1"/>
-    </row>
-    <row r="20" spans="1:12" ht="51">
-      <c r="A20" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="I20" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12" ht="38.25">
+      <c r="A21" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="K20" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="L20" s="1"/>
-    </row>
-    <row r="21" spans="1:12" ht="25.5">
-      <c r="A21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="I21" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>88</v>
+        <v>47</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>89</v>
+        <v>26</v>
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="25.5">
+    <row r="22" spans="1:12" ht="51">
       <c r="A22" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>27</v>
+        <v>80</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>28</v>
+        <v>81</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>29</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="I22" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="38.25">
+    <row r="23" spans="1:12" ht="25.5">
       <c r="A23" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C23" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>40</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="I23" s="2" t="b">
         <v>1</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>26</v>
+        <v>95</v>
       </c>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="51">
+    <row r="24" spans="1:12" ht="25.5">
       <c r="A24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="G24" s="1"/>
       <c r="H24" s="1" t="s">
-        <v>74</v>
+        <v>30</v>
       </c>
       <c r="I24" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>106</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
       <c r="L24" s="1"/>
     </row>
     <row r="25" spans="1:12" ht="25.5">
       <c r="A25" s="1" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="L25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" ht="38.25">
+      <c r="A26" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I25" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="L25" s="1"/>
-    </row>
-    <row r="26" spans="1:12" ht="25.5">
-      <c r="A26" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C26" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="G26" s="1"/>
+      <c r="G26" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="H26" s="1" t="s">
-        <v>30</v>
+        <v>63</v>
       </c>
       <c r="I26" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="25.5">
+    <row r="27" spans="1:12" ht="38.25">
       <c r="A27" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="G27" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="I27" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J27" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>120</v>
-      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="38.25">
-      <c r="A28" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I28" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-    </row>
-    <row r="29" spans="1:12" ht="38.25">
-      <c r="A29" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I29" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-    </row>
-    <row r="30" spans="1:12" ht="23.55" customHeight="1"/>
+    <row r="28" spans="1:12" ht="23.55" customHeight="1"/>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="1" footer="1"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>